<commit_message>
start adding Marquis-esque moderate hw plot
</commit_message>
<xml_diff>
--- a/data/bare-land-data.xlsx
+++ b/data/bare-land-data.xlsx
@@ -586,16 +586,14 @@
   </sheetPr>
   <dimension ref="A1:F321"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A232" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A250" activeCellId="0" sqref="A250"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C213" activeCellId="0" sqref="C213:C248"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="2" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="9.2"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5452,12 +5450,12 @@
   <dimension ref="A1:E55"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F20" activeCellId="0" sqref="F20"/>
+      <selection pane="topLeft" activeCell="F20" activeCellId="1" sqref="C213:C248 F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="2" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1" style="2" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="10.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>